<commit_message>
Produto4 faltando projeçoes, propostas redução e 2a parte ed amb
</commit_message>
<xml_diff>
--- a/produtos/prodquatro/tabelasP4.xlsx
+++ b/produtos/prodquatro/tabelasP4.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TalitaGuerra\Documents\GitHub\talita_PMGIRS\latex_PMGIRS\produtos\prodquatro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00036FB-7D18-4FCD-84B8-B7F0DD74F190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B108B347-47B1-4B1B-88B1-B09274613C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D9246B6E-7205-43C1-9B51-7C5EA50DADD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D9246B6E-7205-43C1-9B51-7C5EA50DADD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="proj_pop" sheetId="2" r:id="rId2"/>
     <sheet name="proj_rs" sheetId="3" r:id="rId3"/>
+    <sheet name="grav_comum_media" sheetId="4" r:id="rId4"/>
+    <sheet name="grav_seletiva_media" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t>Objetivos</t>
   </si>
@@ -44,123 +46,259 @@
     <t>Prazos</t>
   </si>
   <si>
-    <t>Enviar para aterro apenas o que for considerado rejeito/Diminuir em X % o que for destinado a aterro</t>
-  </si>
-  <si>
-    <t>Promover gestão participativa da comunidade</t>
-  </si>
-  <si>
-    <t>Criar e manter canais de comunicação abertos</t>
-  </si>
-  <si>
-    <t>Educação ambiental</t>
-  </si>
-  <si>
     <t>Fomentar ações que possibilitem geração de renda via resíduos</t>
   </si>
   <si>
-    <t>Incentivos a empresas que utilizem, no mínimo, o 3R</t>
-  </si>
-  <si>
     <t>Universalizar os serviços de limpeza urbana e manejo de RS</t>
   </si>
   <si>
-    <t>Compostar X % dos orgânicos no município</t>
-  </si>
-  <si>
-    <t>Coleta seletiva - programa de pontos</t>
+    <t>Projeção populacional</t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Pop. Urbana</t>
+  </si>
+  <si>
+    <t>Pop. Rural</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Fonte: Fundação Seade</t>
+  </si>
+  <si>
+    <t>Fonte: IBGE</t>
+  </si>
+  <si>
+    <t>Projeção da geração de resíduos sólidos</t>
+  </si>
+  <si>
+    <t>Resíduos comuns</t>
+  </si>
+  <si>
+    <t>Resíduos de Serviços de Saúde</t>
+  </si>
+  <si>
+    <t>(t)</t>
+  </si>
+  <si>
+    <t>Dados de geração (t)</t>
+  </si>
+  <si>
+    <t>Dados de coleta (t)</t>
+  </si>
+  <si>
+    <t>Pop. Total</t>
+  </si>
+  <si>
+    <t>Per capta RC (kg/hab.dia)</t>
+  </si>
+  <si>
+    <t>Quantidade RC</t>
+  </si>
+  <si>
+    <t>Per capta RSS (kg/hab.dia)</t>
+  </si>
+  <si>
+    <t>Quantidade RSS total</t>
+  </si>
+  <si>
+    <t>Quantidade RSS (A e E)</t>
+  </si>
+  <si>
+    <t>plano</t>
+  </si>
+  <si>
+    <t>estimado igual ao último valor (t)</t>
+  </si>
+  <si>
+    <t>projetado pelo último valor (t)</t>
+  </si>
+  <si>
+    <t>Tipo de resíduo</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Orgânico</t>
+  </si>
+  <si>
+    <t>Tecido</t>
+  </si>
+  <si>
+    <t>Higiênicos</t>
+  </si>
+  <si>
+    <t>Plástico fino</t>
+  </si>
+  <si>
+    <t>Papel/papelão</t>
+  </si>
+  <si>
+    <t>Plástico duro</t>
+  </si>
+  <si>
+    <t>Metais mistos</t>
+  </si>
+  <si>
+    <t>Madeira</t>
+  </si>
+  <si>
+    <t>Pneu</t>
+  </si>
+  <si>
+    <t>Vidro</t>
   </si>
   <si>
     <r>
-      <t>Logística reversa pós-consumo</t>
+      <t>Fonte:</t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC45911"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> Elaborado pelos autores.</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- parcerias, programa de pontos</t>
-    </r>
-  </si>
-  <si>
-    <t>Projeção populacional</t>
-  </si>
-  <si>
-    <t>Ano</t>
-  </si>
-  <si>
-    <t>Pop. Urbana</t>
-  </si>
-  <si>
-    <t>Pop. Rural</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Fonte: Fundação Seade</t>
-  </si>
-  <si>
-    <t>Fonte: IBGE</t>
-  </si>
-  <si>
-    <t>Projeção da geração de resíduos sólidos</t>
-  </si>
-  <si>
-    <t>Resíduos comuns</t>
-  </si>
-  <si>
-    <t>Resíduos de Serviços de Saúde</t>
-  </si>
-  <si>
-    <t>(t)</t>
-  </si>
-  <si>
-    <t>Dados de geração (t)</t>
-  </si>
-  <si>
-    <t>Dados de coleta (t)</t>
-  </si>
-  <si>
-    <t>Pop. Total</t>
-  </si>
-  <si>
-    <t>Per capta RC (kg/hab.dia)</t>
-  </si>
-  <si>
-    <t>Quantidade RC</t>
-  </si>
-  <si>
-    <t>Per capta RSS (kg/hab.dia)</t>
-  </si>
-  <si>
-    <t>Quantidade RSS total</t>
-  </si>
-  <si>
-    <t>Quantidade RSS (A e E)</t>
-  </si>
-  <si>
-    <t>plano</t>
-  </si>
-  <si>
-    <t>estimado igual ao último valor (t)</t>
-  </si>
-  <si>
-    <t>projetado pelo último valor (t)</t>
+  </si>
+  <si>
+    <t>Papelão</t>
+  </si>
+  <si>
+    <t>Papel</t>
+  </si>
+  <si>
+    <t>Tetra pak</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Isopor</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Tabela 1: Composição gravimétrica da coleta comum.</t>
+  </si>
+  <si>
+    <t>Tabela 2: Composição gravimétrica dos resíduos da coleta seletiva</t>
+  </si>
+  <si>
+    <t>Composteiras em todos os prédios públicos</t>
+  </si>
+  <si>
+    <t>Recipientes para segregação correta em todos os prédios públicos</t>
+  </si>
+  <si>
+    <t>Ações</t>
+  </si>
+  <si>
+    <t>Compostagem</t>
+  </si>
+  <si>
+    <t>2020-2040</t>
+  </si>
+  <si>
+    <t>Aumentar em 60 % a qualidade da segregação dos RS comum</t>
+  </si>
+  <si>
+    <t>Incentivo à compostagem doméstica e coletiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar pontos de recebimento de roupas e tecidos </t>
+  </si>
+  <si>
+    <t>Melhorar a segregação na fonte de geração</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coleta seletiva </t>
+  </si>
+  <si>
+    <t>Divulgação constante</t>
+  </si>
+  <si>
+    <t>Incentivo a programa de pontos</t>
+  </si>
+  <si>
+    <t>Expandir os pontos de coleta de óleo de cozinha usado</t>
+  </si>
+  <si>
+    <t>Regularizar terreno para disposição de RCC</t>
+  </si>
+  <si>
+    <t>Reduzir em 30 % o que for destinado a aterro (como RSU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduzir a geração de RSU </t>
+  </si>
+  <si>
+    <t>Compostar, localmente, 35 % dos orgânicos gerados no município</t>
+  </si>
+  <si>
+    <t>Ponto de armazenagem de matéria seca para compostagem</t>
+  </si>
+  <si>
+    <t>Afixar nos prédios públicos as categorias de resíduos e formas de descarte</t>
+  </si>
+  <si>
+    <t>Correção do gerenciamento dos RCC</t>
+  </si>
+  <si>
+    <t>Contatar o órgão ambiental competente para verificar o procedimento</t>
+  </si>
+  <si>
+    <t>Criar meios de reaproveitamento de RCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação de pontos de entrega, armazenagem e troca de RCC </t>
+  </si>
+  <si>
+    <t>Estimular intercâmbio de materiais RCC entre os munícipes</t>
+  </si>
+  <si>
+    <t>Manter as redes sociais ativas</t>
+  </si>
+  <si>
+    <t>Promover, periodicamente, rodas de conversa com munícipes para melhoria do diálogo com a sociedade</t>
+  </si>
+  <si>
+    <t>Incentivar o engajamento contínuo da rede escolar presente no município</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promover, periodicamente, oficinas participativas com a sociedade </t>
+  </si>
+  <si>
+    <t>Promover gestão participativa da comunidade (destaca-se aqui a importância de valorizar o conhecimento da população local)</t>
+  </si>
+  <si>
+    <t>Criar e manter canais de comunicação abertos com ênfase na Educação Ambiental</t>
+  </si>
+  <si>
+    <t>Incentivos a empresas que utilizem, no mínimo, o princípio dos 3R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dialogar com os catadores autônomos </t>
+  </si>
+  <si>
+    <t>Organizar uma associação ou cooperativa de catadores de materiais reutilizáveis ou recicláveis, respeitando as capacidades de liderança dos próprios cooperados</t>
+  </si>
+  <si>
+    <t>Incentivar a criação/instalação de empresas que façam o beneficiamento (agregar valor) aos resíduos provenientes da coleta seletiva</t>
+  </si>
+  <si>
+    <t>Abatimento de impostos, linhas de crédito diferenciadas</t>
+  </si>
+  <si>
+    <t>Incentivar a implantação da logística reversa pós-consumo - parcerias, programa de pontos</t>
   </si>
 </sst>
 </file>
@@ -170,7 +308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,8 +364,74 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFED7D31"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC45911"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFC45911"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFED7D31"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,8 +480,14 @@
         <bgColor indexed="43"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -403,11 +613,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -552,9 +814,78 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -574,6 +905,60 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4020,86 +4405,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718EFAB6-48B5-4E29-8069-7AD377A0D5E6}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="83" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="83" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="84"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="86">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="84"/>
+      <c r="B4" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="84"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="86">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="84"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="84"/>
+      <c r="B7" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="86">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="84"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="86">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="84"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="84"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="86">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="84"/>
+      <c r="B11" s="93" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="86">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="84"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="86">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="84"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="86">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="84"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="84"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="99" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="84"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="99" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="B18" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="99"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="91"/>
+      <c r="B19" s="100" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="99"/>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="92"/>
+      <c r="B20" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="86"/>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B21" s="85"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="86"/>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="90" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="86"/>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="91"/>
+      <c r="B23" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="86"/>
+    </row>
+    <row r="24" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="92"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="86"/>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="88"/>
+      <c r="B25" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="87"/>
+      <c r="D25" s="86"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="88"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="86"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="88"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="86"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="88"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="86"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="88"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="86"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="88"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="86"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="88"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="86"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="88"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="86"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="88"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="86"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="88"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="86"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="88"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="86"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="88"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="86"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="88"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="87"/>
+      <c r="D37" s="86"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="88"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="86"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="88"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="86"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="88"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="86"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="88"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="86"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="88"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="86"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="88"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="86"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="88"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="87"/>
+      <c r="D44" s="86"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="88"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="86"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="88"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="86"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="88"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="87"/>
+      <c r="D47" s="86"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="88"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="87"/>
+      <c r="D48" s="86"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="88"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="86"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="88"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="86"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="88"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
+  <mergeCells count="10">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4122,13 +4874,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="F1" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -4136,28 +4888,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4293,13 +5045,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -4315,7 +5067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07DF259-C2BD-443A-A838-1369E1B2D22A}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+    <sheetView topLeftCell="E13" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -4331,31 +5083,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
-      <c r="C2" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="C2" s="81" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="82"/>
+      <c r="E2" s="81" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
       <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4363,42 +5115,42 @@
       <c r="B3" s="48"/>
       <c r="C3" s="49"/>
       <c r="D3" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="51"/>
+        <v>15</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="76"/>
       <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="I4" s="30"/>
     </row>
@@ -4520,8 +5272,8 @@
       <c r="H8" s="36">
         <v>1.5329999999999999</v>
       </c>
-      <c r="I8" s="52" t="s">
-        <v>32</v>
+      <c r="I8" s="77" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4552,7 +5304,7 @@
       <c r="H9" s="33">
         <v>1.5</v>
       </c>
-      <c r="I9" s="52"/>
+      <c r="I9" s="77"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
@@ -4582,7 +5334,7 @@
       <c r="H10" s="36">
         <v>1.4</v>
       </c>
-      <c r="I10" s="52"/>
+      <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
@@ -4612,7 +5364,7 @@
       <c r="H11" s="33">
         <v>1.7</v>
       </c>
-      <c r="I11" s="53"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
@@ -4643,7 +5395,7 @@
         <v>1.7</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4675,7 +5427,7 @@
         <v>1.7223753952942553</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5320,4 +6072,257 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1327F0BA-B96C-4DA4-BFE4-1C73427F6980}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="75" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="54">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="55">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="57">
+        <v>0.128</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="58">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="54">
+        <v>0.13</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="55">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="57">
+        <v>0.114</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="58">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="54">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="55">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="57">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="58"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="71"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495DC845-A077-4B21-A97B-DB4B8014C503}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="65">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="66">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="68">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="69">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="65">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C5" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="66">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="68">
+        <v>0.107</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="69">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="65">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="66">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="68">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="69">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
versao enviada para avaliacao Lucas
</commit_message>
<xml_diff>
--- a/produtos/prodquatro/tabelasP4.xlsx
+++ b/produtos/prodquatro/tabelasP4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TalitaGuerra\Documents\GitHub\talita_PMGIRS\latex_PMGIRS\produtos\prodquatro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B108B347-47B1-4B1B-88B1-B09274613C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D1E040-DBE3-4165-B822-298A937A581F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D9246B6E-7205-43C1-9B51-7C5EA50DADD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D9246B6E-7205-43C1-9B51-7C5EA50DADD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -886,6 +886,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -905,60 +959,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2035,7 +2035,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" sz="1200" b="0" i="0" baseline="0"/>
-              <a:t>Quantidade RSS</a:t>
+              <a:t>Quantidade RSS (A e E)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2074,26 +2074,26 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:idx val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>proj_rs!$F$4</c:f>
+              <c:f>proj_rs!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Quantidade RSS total</c:v>
+                  <c:v>Quantidade RSS (A e E)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -2101,78 +2101,98 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>proj_rs!$A$5:$A$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>proj_rs!$A$14:$A$34</c:f>
+              <c:f>proj_rs!$A$5:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2020</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
                   <c:v>2021</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="12">
                   <c:v>2023</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="13">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="14">
                   <c:v>2025</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="15">
                   <c:v>2026</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="16">
                   <c:v>2027</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="17">
                   <c:v>2028</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="18">
                   <c:v>2029</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
                   <c:v>2030</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="20">
                   <c:v>2031</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="21">
                   <c:v>2032</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="22">
                   <c:v>2033</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="23">
                   <c:v>2034</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="24">
                   <c:v>2035</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="25">
                   <c:v>2036</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="26">
                   <c:v>2037</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="27">
                   <c:v>2038</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="28">
                   <c:v>2039</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="29">
                   <c:v>2040</c:v>
                 </c:pt>
               </c:numCache>
@@ -2180,86 +2200,106 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>proj_rs!$F$5:$F$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>proj_rs!$F$14:$F$34</c:f>
+              <c:f>proj_rs!$H$5:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>47.9884835408022</c:v>
+                  <c:v>1.5329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.829405095651104</c:v>
+                  <c:v>1.5329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.5379075765157</c:v>
+                  <c:v>1.5329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.255735365072212</c:v>
+                  <c:v>1.5329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.98301120099471</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.719859439456471</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.466406072393198</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>58.222778750046132</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58.989106802788626</c:v>
+                  <c:v>1.7223753952942553</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59.765521263240061</c:v>
+                  <c:v>1.745045295479436</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60.552154888670785</c:v>
+                  <c:v>1.7680135768281025</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61.349142183701943</c:v>
+                  <c:v>1.7912841666323021</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>62.156619423304186</c:v>
+                  <c:v>1.8148610438750892</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>62.974724676098901</c:v>
+                  <c:v>1.8387482399108832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63.803597827966314</c:v>
+                  <c:v>1.8629498391547787</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>64.605788311244879</c:v>
+                  <c:v>1.8874699797809302</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>65.41863514834364</c:v>
+                  <c:v>1.9123128544301293</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>66.231481985442414</c:v>
+                  <c:v>1.9374827109266939</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>67.04432882254126</c:v>
+                  <c:v>1.9629838530047941</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>67.857175659640035</c:v>
+                  <c:v>1.9888206410443368</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>68.670022496738795</c:v>
+                  <c:v>2.0149974928165371</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0415188842393039</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0683893501425632</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.0956134850436623</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.1219612342546856</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1486589887871519</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.1753567433196186</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2020544978520884</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.2287522523845551</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.2554500069170214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CECB-47CA-B649-AF424FF936AF}"/>
+              <c16:uniqueId val="{00000001-CECB-47CA-B649-AF424FF936AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2274,214 +2314,261 @@
         <c:gapWidth val="150"/>
         <c:axId val="1084517615"/>
         <c:axId val="1088530799"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>proj_rs!$F$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Quantidade RSS total</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>proj_rs!$A$5:$A$34</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="30"/>
+                      <c:pt idx="0">
+                        <c:v>2011</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2012</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2013</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2014</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2015</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2017</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2023</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2024</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2025</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2026</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>2027</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2028</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>2029</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>2030</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2031</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>2032</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2033</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>2034</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>2035</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>2036</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2037</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>2038</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>2039</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>2040</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>proj_rs!$F$5:$F$34</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.000</c:formatCode>
+                      <c:ptCount val="30"/>
+                      <c:pt idx="0">
+                        <c:v>42.658279999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43.22210307622079</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>43.790992277267542</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44.36736919640375</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44.951332386954157</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>45.542981699402134</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>46.142418298462808</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>46.749744680381042</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>47.365064690456947</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>47.9884835408022</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>53.829405095651104</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>54.5379075765157</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>55.255735365072212</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>55.98301120099471</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>56.719859439456471</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>57.466406072393198</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>58.222778750046132</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>58.989106802788626</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>59.765521263240061</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>60.552154888670785</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>61.349142183701943</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>62.156619423304186</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>62.974724676098901</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>63.803597827966314</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>64.605788311244879</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>65.41863514834364</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>66.231481985442414</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>67.04432882254126</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>67.857175659640035</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>68.670022496738795</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-CECB-47CA-B649-AF424FF936AF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>proj_rs!$H$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Quantidade RSS (A e E)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>proj_rs!$A$5:$A$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>proj_rs!$A$14:$A$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2024</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2026</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2027</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2028</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2029</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2031</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2032</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2033</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2034</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2035</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2036</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2037</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2038</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2039</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2040</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>proj_rs!$H$5:$H$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>proj_rs!$H$14:$H$34</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>1.745045295479436</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7680135768281025</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7912841666323021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8148610438750892</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8387482399108832</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.8629498391547787</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8874699797809302</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.9123128544301293</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.9374827109266939</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.9629838530047941</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.9888206410443368</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0149974928165371</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.0415188842393039</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.0683893501425632</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.0956134850436623</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.1219612342546856</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.1486589887871519</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.1753567433196186</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.2020544978520884</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.2287522523845551</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.2554500069170214</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CECB-47CA-B649-AF424FF936AF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1082626703"/>
-        <c:axId val="1088474639"/>
-      </c:lineChart>
       <c:catAx>
         <c:axId val="1084517615"/>
         <c:scaling>
@@ -2596,6 +2683,8 @@
         <c:axId val="1088530799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2675,7 +2764,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2706,127 +2795,8 @@
         <c:crossAx val="1084517615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
-      <c:valAx>
-        <c:axId val="1088474639"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Toneladas</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1082626703"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="1082626703"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1088474639"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2835,37 +2805,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -4407,7 +4346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718EFAB6-48B5-4E29-8069-7AD377A0D5E6}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -4419,426 +4358,426 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="76" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="87" t="s">
+      <c r="A3" s="90"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="78">
         <v>2022</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="84"/>
-      <c r="B4" s="93" t="s">
+      <c r="A4" s="90"/>
+      <c r="B4" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="87" t="s">
+      <c r="A5" s="90"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="78">
         <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="87" t="s">
+      <c r="A6" s="90"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="95" t="s">
+      <c r="A7" s="90"/>
+      <c r="B7" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="86">
+      <c r="D7" s="78">
         <v>2024</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
-      <c r="B8" s="97"/>
-      <c r="C8" s="87" t="s">
+      <c r="A8" s="90"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="86">
+      <c r="D8" s="78">
         <v>2028</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="97"/>
-      <c r="C9" s="87" t="s">
+      <c r="A9" s="90"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="84"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="87" t="s">
+      <c r="A10" s="90"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="86">
+      <c r="D10" s="78">
         <v>2022</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="84"/>
-      <c r="B11" s="93" t="s">
+      <c r="A11" s="90"/>
+      <c r="B11" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="78">
         <v>2028</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="87" t="s">
+      <c r="A12" s="90"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="78">
         <v>2022</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="84"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="87" t="s">
+      <c r="A13" s="90"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="78">
         <v>2022</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="87" t="s">
+      <c r="A15" s="90"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="87" t="s">
+      <c r="A16" s="90"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="99" t="s">
+      <c r="D16" s="82" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="84"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="87" t="s">
+      <c r="A17" s="90"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="82" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="100" t="s">
+      <c r="B18" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="87" t="s">
+      <c r="C18" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="99"/>
+      <c r="D18" s="82"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="91"/>
-      <c r="B19" s="100" t="s">
+      <c r="A19" s="85"/>
+      <c r="B19" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="87" t="s">
+      <c r="C19" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="99"/>
+      <c r="D19" s="82"/>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="85" t="s">
+      <c r="A20" s="86"/>
+      <c r="B20" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="86"/>
+      <c r="D20" s="78"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="88" t="s">
+      <c r="A21" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="85"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="86"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="78"/>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="86"/>
+      <c r="D22" s="78"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="91"/>
-      <c r="B23" s="93" t="s">
+      <c r="A23" s="85"/>
+      <c r="B23" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="86"/>
+      <c r="D23" s="78"/>
     </row>
     <row r="24" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="94"/>
-      <c r="C24" s="87" t="s">
+      <c r="A24" s="86"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="86"/>
+      <c r="D24" s="78"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
-      <c r="B25" s="85" t="s">
+      <c r="A25" s="80"/>
+      <c r="B25" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="87"/>
-      <c r="D25" s="86"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="78"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="88"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="86"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="78"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="86"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="78"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="86"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="78"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="88"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="86"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="78"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="88"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="86"/>
+      <c r="A30" s="80"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="78"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="86"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="78"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="86"/>
+      <c r="A32" s="80"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="78"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="88"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="86"/>
+      <c r="A33" s="80"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="78"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="88"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="86"/>
+      <c r="A34" s="80"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="78"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="88"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="86"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="78"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="88"/>
-      <c r="B36" s="85"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="86"/>
+      <c r="A36" s="80"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="78"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="88"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="86"/>
+      <c r="A37" s="80"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="78"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="88"/>
-      <c r="B38" s="89"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="86"/>
+      <c r="A38" s="80"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="78"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="88"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="86"/>
+      <c r="A39" s="80"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="78"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="87"/>
-      <c r="D40" s="86"/>
+      <c r="A40" s="80"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="78"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="88"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="87"/>
-      <c r="D41" s="86"/>
+      <c r="A41" s="80"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="78"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="88"/>
-      <c r="B42" s="85"/>
-      <c r="C42" s="87"/>
-      <c r="D42" s="86"/>
+      <c r="A42" s="80"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="78"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="88"/>
-      <c r="B43" s="85"/>
-      <c r="C43" s="87"/>
-      <c r="D43" s="86"/>
+      <c r="A43" s="80"/>
+      <c r="B43" s="77"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="78"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="87"/>
-      <c r="D44" s="86"/>
+      <c r="A44" s="80"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="78"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="88"/>
-      <c r="B45" s="85"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="86"/>
+      <c r="A45" s="80"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="78"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="88"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="87"/>
-      <c r="D46" s="86"/>
+      <c r="A46" s="80"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="78"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="88"/>
-      <c r="B47" s="85"/>
-      <c r="C47" s="87"/>
-      <c r="D47" s="86"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="78"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="88"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="87"/>
-      <c r="D48" s="86"/>
+      <c r="A48" s="80"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="78"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="88"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="86"/>
+      <c r="A49" s="80"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="78"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="88"/>
-      <c r="B50" s="85"/>
-      <c r="C50" s="87"/>
-      <c r="D50" s="86"/>
+      <c r="A50" s="80"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="78"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="88"/>
-      <c r="B51" s="85"/>
-      <c r="C51" s="87"/>
-      <c r="D51" s="86"/>
+      <c r="A51" s="80"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4863,7 +4802,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="F1" sqref="F1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5067,8 +5006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07DF259-C2BD-443A-A838-1369E1B2D22A}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="M6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5083,31 +5022,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="80"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="98"/>
       <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="81" t="s">
+      <c r="D2" s="100"/>
+      <c r="E2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5117,14 +5056,14 @@
       <c r="D3" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="76"/>
+      <c r="H3" s="94"/>
       <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
@@ -5272,7 +5211,7 @@
       <c r="H8" s="36">
         <v>1.5329999999999999</v>
       </c>
-      <c r="I8" s="77" t="s">
+      <c r="I8" s="95" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5304,7 +5243,7 @@
       <c r="H9" s="33">
         <v>1.5</v>
       </c>
-      <c r="I9" s="77"/>
+      <c r="I9" s="95"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
@@ -5334,7 +5273,7 @@
       <c r="H10" s="36">
         <v>1.4</v>
       </c>
-      <c r="I10" s="77"/>
+      <c r="I10" s="95"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
@@ -5364,7 +5303,7 @@
       <c r="H11" s="33">
         <v>1.7</v>
       </c>
-      <c r="I11" s="78"/>
+      <c r="I11" s="96"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="22">

</xml_diff>

<commit_message>
tabela de metas P4
</commit_message>
<xml_diff>
--- a/produtos/prodquatro/tabelasP4.xlsx
+++ b/produtos/prodquatro/tabelasP4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TalitaGuerra\Documents\GitHub\talita_PMGIRS\latex_PMGIRS\produtos\prodquatro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D1E040-DBE3-4165-B822-298A937A581F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44921154-B0D8-478F-9E9E-621A214EF155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D9246B6E-7205-43C1-9B51-7C5EA50DADD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D9246B6E-7205-43C1-9B51-7C5EA50DADD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="111">
   <si>
     <t>Objetivos</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Fomentar ações que possibilitem geração de renda via resíduos</t>
-  </si>
-  <si>
-    <t>Universalizar os serviços de limpeza urbana e manejo de RS</t>
   </si>
   <si>
     <t>Projeção populacional</t>
@@ -214,33 +211,21 @@
     <t>Incentivo à compostagem doméstica e coletiva</t>
   </si>
   <si>
-    <t xml:space="preserve">Criar pontos de recebimento de roupas e tecidos </t>
-  </si>
-  <si>
     <t>Melhorar a segregação na fonte de geração</t>
   </si>
   <si>
-    <t xml:space="preserve">Coleta seletiva </t>
-  </si>
-  <si>
     <t>Divulgação constante</t>
   </si>
   <si>
     <t>Incentivo a programa de pontos</t>
   </si>
   <si>
-    <t>Expandir os pontos de coleta de óleo de cozinha usado</t>
-  </si>
-  <si>
     <t>Regularizar terreno para disposição de RCC</t>
   </si>
   <si>
     <t>Reduzir em 30 % o que for destinado a aterro (como RSU)</t>
   </si>
   <si>
-    <t xml:space="preserve">Reduzir a geração de RSU </t>
-  </si>
-  <si>
     <t>Compostar, localmente, 35 % dos orgânicos gerados no município</t>
   </si>
   <si>
@@ -259,9 +244,6 @@
     <t>Criar meios de reaproveitamento de RCC</t>
   </si>
   <si>
-    <t xml:space="preserve">Criação de pontos de entrega, armazenagem e troca de RCC </t>
-  </si>
-  <si>
     <t>Estimular intercâmbio de materiais RCC entre os munícipes</t>
   </si>
   <si>
@@ -274,9 +256,6 @@
     <t>Incentivar o engajamento contínuo da rede escolar presente no município</t>
   </si>
   <si>
-    <t xml:space="preserve">Promover, periodicamente, oficinas participativas com a sociedade </t>
-  </si>
-  <si>
     <t>Promover gestão participativa da comunidade (destaca-se aqui a importância de valorizar o conhecimento da população local)</t>
   </si>
   <si>
@@ -286,9 +265,6 @@
     <t>Incentivos a empresas que utilizem, no mínimo, o princípio dos 3R</t>
   </si>
   <si>
-    <t xml:space="preserve">Dialogar com os catadores autônomos </t>
-  </si>
-  <si>
     <t>Organizar uma associação ou cooperativa de catadores de materiais reutilizáveis ou recicláveis, respeitando as capacidades de liderança dos próprios cooperados</t>
   </si>
   <si>
@@ -298,7 +274,112 @@
     <t>Abatimento de impostos, linhas de crédito diferenciadas</t>
   </si>
   <si>
-    <t>Incentivar a implantação da logística reversa pós-consumo - parcerias, programa de pontos</t>
+    <t>Reduzir a geração de RSU</t>
+  </si>
+  <si>
+    <t>Criar pontos de recebimento de roupas e tecidos</t>
+  </si>
+  <si>
+    <t>Coleta seletiva</t>
+  </si>
+  <si>
+    <t>Expandir os pontos de coleta de óleo de cozinha usado (centros comunitários, escolas e mercados, em cada bairro)</t>
+  </si>
+  <si>
+    <t>Priorização da educação ambiental nos currículos escolares</t>
+  </si>
+  <si>
+    <t>Promover, periodicamente, oficinas participativas com a sociedade</t>
+  </si>
+  <si>
+    <t>Dialogar com os catadores autônomos</t>
+  </si>
+  <si>
+    <t>Consulta ao Programa Pró-Catador para obtenção de recursos para a infraestrutura</t>
+  </si>
+  <si>
+    <t>Estudo sobre possíveis terrenos públicos onde a cooperativa/associação poderá ser instalada</t>
+  </si>
+  <si>
+    <t>Incentivar a criação por meio de abatimento de impostos ou linhas de crédito diferenciadas</t>
+  </si>
+  <si>
+    <t>Construção da cooperativa/associação</t>
+  </si>
+  <si>
+    <t>Melhoria dos serviços de limpeza urbana e manejo de RS</t>
+  </si>
+  <si>
+    <t>Padronização e instalação de "lixeiras"</t>
+  </si>
+  <si>
+    <t>Definição de modelo mais ergonômico aos coletores (com porta articulada, por exemplo), duradouro e com separação para orgânico e reciclável. Preferencialmente com cobertura contra chuvas.</t>
+  </si>
+  <si>
+    <t>Otimizar as rotas dos caminhões coletores</t>
+  </si>
+  <si>
+    <t>Manter o controle quantitativo da movimentação dos resíduos</t>
+  </si>
+  <si>
+    <t>Interromper a disposição de RCC para o "bota-fora" municipal</t>
+  </si>
+  <si>
+    <t>Criação de pontos de entrega, armazenagem e troca de RCC</t>
+  </si>
+  <si>
+    <t>Logística Reversa</t>
+  </si>
+  <si>
+    <t>Preencher correta e regularmente os formulários do SNIS</t>
+  </si>
+  <si>
+    <t>Criar um padrão de coleta dos dados para evitar futuras interpretações ambíguas</t>
+  </si>
+  <si>
+    <t>Verificar os dados solicitados</t>
+  </si>
+  <si>
+    <t>Manter o registro das informações em meio digital de modo acessivel ao responsável na gestão corrente</t>
+  </si>
+  <si>
+    <t>Evitar estimar dados, utilizar valores concretos (exemplo: valores de contratos, pesos e medidas coletados, etc.)</t>
+  </si>
+  <si>
+    <t>Utilizar valores atuais (correntes no ano)</t>
+  </si>
+  <si>
+    <t>Aprimorar anualmente o preenchimeto</t>
+  </si>
+  <si>
+    <t>Coletar durante o ano os dados solicitados</t>
+  </si>
+  <si>
+    <t>Verificar as dificuldades enfrentadas para o preenchimento (ausência de dados, dificuldade de coleta, etc) e montar uma estratégia para solucioná-las no ano seguinte</t>
+  </si>
+  <si>
+    <t>Estudo para identificar possíveis rotas mais eficientes e manter o padrão desse deslocamento para geraçao de dados consistentes a respeito</t>
+  </si>
+  <si>
+    <t>Manutenção preventiva dos equipamentos</t>
+  </si>
+  <si>
+    <t>Criar uma escala de manutenção preventiva</t>
+  </si>
+  <si>
+    <t>Registro de dados de movimentação dos resíduos</t>
+  </si>
+  <si>
+    <t>Incentivar a implantação da logística reversa pós-consumo</t>
+  </si>
+  <si>
+    <t>Verificar a possibilidade do estabelecimento de parcerias e/ou programa de pontos com empreendimentos</t>
+  </si>
+  <si>
+    <t>2022-2024</t>
+  </si>
+  <si>
+    <t>Inserir pontos de coleta em lugares de fácil acesso</t>
   </si>
 </sst>
 </file>
@@ -431,7 +512,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,7 +563,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,7 +742,9 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -660,20 +755,15 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -886,60 +976,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -961,6 +997,49 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4344,449 +4423,897 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718EFAB6-48B5-4E29-8069-7AD377A0D5E6}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="82" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="94" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G3" s="88"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="94" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="84"/>
+      <c r="B4" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="88"/>
+      <c r="H4" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="84"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G5" s="88"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="88"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="84"/>
+      <c r="B7" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="82" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="82">
+        <v>2024</v>
+      </c>
+      <c r="G7" s="88"/>
+      <c r="H7" s="91" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="95">
+        <v>2024</v>
+      </c>
+      <c r="L7" s="96"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="84"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="82" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="82">
+        <v>2028</v>
+      </c>
+      <c r="G8" s="88"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="95">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="84"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="88"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G10" s="88"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="94" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="84"/>
+      <c r="B11" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="76" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="C11" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="82">
+        <v>2028</v>
+      </c>
+      <c r="G11" s="88"/>
+      <c r="H11" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="95">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="84"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G12" s="88"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="85"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="82" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G13" s="89"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="94" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="94" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="84"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="88"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="84"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="88"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="84"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="88"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="85"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="89"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G19" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="84"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G20" s="88"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="84"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G21" s="88"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="94" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="84"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="82">
+        <v>2024</v>
+      </c>
+      <c r="G22" s="88"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" s="95">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="84"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="82">
+        <v>2024</v>
+      </c>
+      <c r="G23" s="88"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" s="95">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="84"/>
+      <c r="B24" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="88"/>
+      <c r="H24" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="85"/>
+      <c r="B25" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="89"/>
+      <c r="H25" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="82">
+        <v>2020</v>
+      </c>
+      <c r="G26" s="87" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" s="95">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="84"/>
+      <c r="B27" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="82">
+        <v>2024</v>
+      </c>
+      <c r="G27" s="88"/>
+      <c r="H27" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="J27" s="95">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="84"/>
+      <c r="B28" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="82">
+        <v>2020</v>
+      </c>
+      <c r="G28" s="88"/>
+      <c r="H28" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" s="94" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="95">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="85"/>
+      <c r="B29" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="82">
+        <v>2020</v>
+      </c>
+      <c r="G29" s="89"/>
+      <c r="H29" s="90" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="95">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="82">
+        <v>2022</v>
+      </c>
+      <c r="G30" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" s="95">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="84"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="87" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="90"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="79" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="78">
+      <c r="D31" s="82">
+        <v>2020</v>
+      </c>
+      <c r="G31" s="88"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="95">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="84"/>
+      <c r="B32" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="82">
         <v>2022</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="90"/>
-      <c r="B4" s="87" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="78">
+      <c r="G32" s="88"/>
+      <c r="H32" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="95">
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="90"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="79" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="90"/>
-      <c r="B7" s="91" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="78">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="90"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="79" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="78">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="90"/>
-      <c r="B10" s="93"/>
-      <c r="C10" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="78">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="90"/>
-      <c r="B11" s="87" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="85"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="78">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="90"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="78">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="79" t="s">
+      <c r="G33" s="89"/>
+      <c r="H33" s="92"/>
+      <c r="I33" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="78">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="82" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="79" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="82" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="82"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
-      <c r="B19" s="83" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="82"/>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="86"/>
-      <c r="B20" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="78"/>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="80" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="78"/>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="78"/>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="85"/>
-      <c r="B23" s="87" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="78"/>
-    </row>
-    <row r="24" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="79" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="78"/>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="80"/>
-      <c r="B25" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="78"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="80"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="78"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="78"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="78"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="78"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="79"/>
-      <c r="D30" s="78"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="78"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="78"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="80"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="78"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="80"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="78"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="80"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="78"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="80"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="78"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="80"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="78"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="80"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="78"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="80"/>
-      <c r="B39" s="77"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="78"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="80"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="78"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="80"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="78"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="80"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="78"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="80"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="79"/>
-      <c r="D43" s="78"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="80"/>
-      <c r="B44" s="77"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="78"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="80"/>
-      <c r="B45" s="77"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="78"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="80"/>
-      <c r="B46" s="77"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="78"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="80"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="78"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="80"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="78"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="80"/>
-      <c r="B49" s="77"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="78"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="80"/>
-      <c r="B50" s="77"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="78"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="80"/>
-      <c r="B51" s="77"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="78"/>
+      <c r="J33" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="83" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="82" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="I34" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="J34" s="95" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="85"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="89"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="J35" s="95" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="82" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="H36" s="91" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="J36" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="84"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="88"/>
+      <c r="H37" s="93"/>
+      <c r="I37" s="94" t="s">
+        <v>97</v>
+      </c>
+      <c r="J37" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="84"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" s="88"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="94" t="s">
+        <v>98</v>
+      </c>
+      <c r="J38" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="84"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="88"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="J39" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="84"/>
+      <c r="B40" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="88"/>
+      <c r="H40" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="I40" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="J40" s="95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="85"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="89"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" s="95" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A20"/>
+  <mergeCells count="36">
+    <mergeCell ref="G36:G41"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="G19:G25"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="G2:G13"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B19:B23"/>
     <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A17"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B4:B6"/>
@@ -4812,189 +5339,189 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1983</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2482</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4465</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2087</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2609</v>
+      </c>
+      <c r="I3" s="7">
+        <v>4696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="13">
+        <v>2069</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2525</v>
+      </c>
+      <c r="D4" s="8">
+        <v>4594</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2025</v>
+      </c>
+      <c r="G4" s="13">
+        <v>2261</v>
+      </c>
+      <c r="H4" s="13">
+        <v>2752</v>
+      </c>
+      <c r="I4" s="8">
+        <v>5013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>2030</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2139</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2544</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4683</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2030</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2449</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2902</v>
+      </c>
+      <c r="I5" s="7">
+        <v>5351</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>2035</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2193</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2544</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4737</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2035</v>
+      </c>
+      <c r="G6" s="13">
+        <v>2653</v>
+      </c>
+      <c r="H6" s="13">
+        <v>3060</v>
+      </c>
+      <c r="I6" s="8">
+        <v>5713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>2040</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2228</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2518</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4746</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2040</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2874</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3225</v>
+      </c>
+      <c r="I7" s="7">
+        <v>6099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>2020</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1983</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2482</v>
-      </c>
-      <c r="D3" s="8">
-        <v>4465</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2020</v>
-      </c>
-      <c r="G3" s="6">
-        <v>2087</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2609</v>
-      </c>
-      <c r="I3" s="8">
-        <v>4696</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>2025</v>
-      </c>
-      <c r="B4" s="14">
-        <v>2069</v>
-      </c>
-      <c r="C4" s="14">
-        <v>2525</v>
-      </c>
-      <c r="D4" s="9">
-        <v>4594</v>
-      </c>
-      <c r="F4" s="11">
-        <v>2025</v>
-      </c>
-      <c r="G4" s="14">
-        <v>2261</v>
-      </c>
-      <c r="H4" s="14">
-        <v>2752</v>
-      </c>
-      <c r="I4" s="9">
-        <v>5013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>2030</v>
-      </c>
-      <c r="B5" s="6">
-        <v>2139</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2544</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4683</v>
-      </c>
-      <c r="F5" s="5">
-        <v>2030</v>
-      </c>
-      <c r="G5" s="6">
-        <v>2449</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2902</v>
-      </c>
-      <c r="I5" s="8">
-        <v>5351</v>
-      </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>2035</v>
-      </c>
-      <c r="B6" s="14">
-        <v>2193</v>
-      </c>
-      <c r="C6" s="14">
-        <v>2544</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4737</v>
-      </c>
-      <c r="F6" s="11">
-        <v>2035</v>
-      </c>
-      <c r="G6" s="14">
-        <v>2653</v>
-      </c>
-      <c r="H6" s="14">
-        <v>3060</v>
-      </c>
-      <c r="I6" s="9">
-        <v>5713</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>2040</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2228</v>
-      </c>
-      <c r="C7" s="6">
-        <v>2518</v>
-      </c>
-      <c r="D7" s="8">
-        <v>4746</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2040</v>
-      </c>
-      <c r="G7" s="6">
-        <v>2874</v>
-      </c>
-      <c r="H7" s="6">
-        <v>3225</v>
-      </c>
-      <c r="I7" s="8">
-        <v>6099</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5006,8 +5533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07DF259-C2BD-443A-A838-1369E1B2D22A}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M6" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView topLeftCell="M6" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5022,982 +5549,982 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="99" t="s">
+      <c r="D2" s="81"/>
+      <c r="E2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="99" t="s">
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="48" t="s">
+      <c r="E3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="F3" s="75"/>
+      <c r="G3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94" t="s">
+      <c r="H3" s="75"/>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="94"/>
-      <c r="I3" s="30"/>
-    </row>
-    <row r="4" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="D4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="F4" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="G4" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="29"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="17">
         <v>2011</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>4174</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>0.48</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <f>(B5*C5)/1000*365</f>
         <v>731.28480000000002</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="36">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="37">
         <f>(E5*B5)*365/1000</f>
         <v>42.658279999999998</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="36">
         <f t="shared" ref="G5:G12" si="0">H5*1000/365/B5</f>
         <v>1.0062290368950647E-3</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="32">
         <v>1.5329999999999999</v>
       </c>
-      <c r="I5" s="30"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>2012</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>4229.1685984560463</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>0.48</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <f t="shared" ref="D6:D34" si="1">(B6*C6)/1000*365</f>
         <v>740.95033844949933</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="34">
         <f t="shared" ref="F6:F34" si="2">(E6*B6)/1000*365</f>
         <v>43.22210307622079</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="33">
         <f t="shared" si="0"/>
         <v>9.9310299464847648E-4</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="35">
         <v>1.5329999999999999</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="29"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="17">
         <v>2013</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>4284.8329038422253</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>0.48</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <f t="shared" si="1"/>
         <v>750.7027247531579</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="31">
         <f t="shared" si="2"/>
         <v>43.790992277267542</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <f t="shared" si="0"/>
         <v>9.8020158411168024E-4</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="32">
         <v>1.5329999999999999</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>2014</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>4341.2298626618149</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>0.48</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <f t="shared" si="1"/>
         <v>760.58347193834993</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="34">
         <f t="shared" si="2"/>
         <v>44.36736919640375</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <f t="shared" si="0"/>
         <v>9.674677759230146E-4</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="35">
         <v>1.5329999999999999</v>
       </c>
-      <c r="I8" s="95" t="s">
-        <v>24</v>
+      <c r="I8" s="76" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="17">
         <v>2015</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>4398.3691180972755</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>0.48</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <f t="shared" si="1"/>
         <v>770.59426949064266</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="30">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <f t="shared" si="2"/>
         <v>44.951332386954157</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="30">
         <f t="shared" si="0"/>
         <v>9.3434382853108285E-4</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="32">
         <v>1.5</v>
       </c>
-      <c r="I9" s="95"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="21">
         <v>2016</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>4456.2604402546112</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>0.48</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <f t="shared" si="1"/>
         <v>780.73682913260791</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="33">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="34">
         <f t="shared" si="2"/>
         <v>45.542981699402134</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="33">
         <f t="shared" si="0"/>
         <v>8.6072537495968571E-4</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="35">
         <v>1.4</v>
       </c>
-      <c r="I10" s="95"/>
+      <c r="I10" s="76"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="17">
         <v>2017</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="18">
         <v>4514.9137278339349</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>0.48</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <f t="shared" si="1"/>
         <v>791.01288511650534</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="30">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="31">
         <f t="shared" si="2"/>
         <v>46.142418298462808</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <f t="shared" si="0"/>
         <v>1.0315887583548203E-3</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="32">
         <v>1.7</v>
       </c>
-      <c r="I11" s="96"/>
+      <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="21">
         <v>2018</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>4574.3390098220198</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>0.48</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <f t="shared" si="1"/>
         <v>801.42419452081788</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="33">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="34">
         <f t="shared" si="2"/>
         <v>46.749744680381042</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="33">
         <f t="shared" si="0"/>
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="35">
         <v>1.7</v>
       </c>
-      <c r="I12" s="26" t="s">
-        <v>25</v>
+      <c r="I12" s="25" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <v>2019</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>4634.5464472071371</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="19">
         <v>0.48</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <f t="shared" si="1"/>
         <v>811.97253755069039</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="30">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <f t="shared" si="2"/>
         <v>47.365064690456947</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="30">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="32">
         <f t="shared" ref="H13:H34" si="3">G13*B13/1000*365</f>
         <v>1.7223753952942553</v>
       </c>
-      <c r="I13" s="27" t="s">
-        <v>26</v>
+      <c r="I13" s="26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="A14" s="21">
         <v>2020</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="22">
         <v>4695.5463347164577</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>0.48</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <f t="shared" si="1"/>
         <v>822.6597178423234</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="33">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="34">
         <f t="shared" si="2"/>
         <v>47.9884835408022</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="33">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="35">
         <f t="shared" si="3"/>
         <v>1.745045295479436</v>
       </c>
-      <c r="I14" s="30"/>
+      <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="17">
         <v>2021</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <v>4757.3491025763242</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>0.51</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <f t="shared" si="1"/>
         <v>885.58053544458278</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <v>3.1E-2</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="31">
         <f t="shared" si="2"/>
         <v>53.829405095651104</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="30">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H15" s="33">
+      <c r="H15" s="32">
         <f t="shared" si="3"/>
         <v>1.7680135768281025</v>
       </c>
-      <c r="I15" s="30"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+      <c r="A16" s="21">
         <v>2022</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>4819.9653182956863</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="23">
         <v>0.51</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="24">
         <f t="shared" si="1"/>
         <v>897.2365440007419</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="33">
         <v>3.1E-2</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="34">
         <f t="shared" si="2"/>
         <v>54.5379075765157</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="33">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="35">
         <f t="shared" si="3"/>
         <v>1.7912841666323021</v>
       </c>
-      <c r="I16" s="30"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+      <c r="A17" s="17">
         <v>2023</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="18">
         <v>4883.4056884730189</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>0.51</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <f t="shared" si="1"/>
         <v>909.04596890925245</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="30">
         <v>3.1E-2</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <f t="shared" si="2"/>
         <v>55.255735365072212</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="30">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="32">
         <f t="shared" si="3"/>
         <v>1.8148610438750892</v>
       </c>
-      <c r="I17" s="30"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="A18" s="21">
         <v>2024</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="22">
         <v>4947.6810606270183</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="23">
         <v>0.51</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="24">
         <f t="shared" si="1"/>
         <v>921.01082943571942</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="33">
         <v>3.1E-2</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="34">
         <f t="shared" si="2"/>
         <v>55.98301120099471</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="33">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="35">
         <f t="shared" si="3"/>
         <v>1.8387482399108832</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="A19" s="17">
         <v>2025</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="18">
         <v>5012.802425051389</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="19">
         <v>0.51</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="27">
         <f t="shared" si="1"/>
         <v>933.13317142331618</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="37">
         <f t="shared" si="2"/>
         <v>56.719859439456471</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="39">
         <f t="shared" si="3"/>
         <v>1.8629498391547787</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
+      <c r="A20" s="21">
         <v>2026</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>5078.7809166940524</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="23">
         <v>0.51</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="28">
         <f t="shared" si="1"/>
         <v>945.41506764259771</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="41">
         <f t="shared" si="2"/>
         <v>57.466406072393198</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="41">
         <f t="shared" si="3"/>
         <v>1.8874699797809302</v>
       </c>
-      <c r="I20" s="30"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="17">
         <v>2027</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="18">
         <v>5145.6278170610813</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <v>0.51</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="27">
         <f t="shared" si="1"/>
         <v>957.85861814592033</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="37">
         <f t="shared" si="2"/>
         <v>58.222778750046132</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="37">
         <f t="shared" si="3"/>
         <v>1.9123128544301293</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+      <c r="A22" s="21">
         <v>2028</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="22">
         <v>5213.3545561457031</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="23">
         <v>0.51</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <f t="shared" si="1"/>
         <v>970.46595062652261</v>
       </c>
-      <c r="E22" s="41">
+      <c r="E22" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="41">
         <f t="shared" si="2"/>
         <v>58.989106802788626</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H22" s="42">
+      <c r="H22" s="41">
         <f t="shared" si="3"/>
         <v>1.9374827109266939</v>
       </c>
-      <c r="I22" s="30"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
+      <c r="A23" s="17">
         <v>2029</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="18">
         <v>5281.972714382684</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="19">
         <v>0.51</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="27">
         <f t="shared" si="1"/>
         <v>983.2392207823367</v>
       </c>
-      <c r="E23" s="37">
+      <c r="E23" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="37">
         <f t="shared" si="2"/>
         <v>59.765521263240061</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="37">
         <f t="shared" si="3"/>
         <v>1.9629838530047941</v>
       </c>
-      <c r="I23" s="30"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+      <c r="A24" s="21">
         <v>2030</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>5351.4940246284386</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="23">
         <v>0.51</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <f t="shared" si="1"/>
         <v>996.18061268458382</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F24" s="42">
+      <c r="F24" s="41">
         <f t="shared" si="2"/>
         <v>60.552154888670785</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H24" s="41">
         <f t="shared" si="3"/>
         <v>1.9888206410443368</v>
       </c>
-      <c r="I24" s="30"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
+      <c r="A25" s="17">
         <v>2031</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="18">
         <v>5421.9303741672065</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="19">
         <v>0.51</v>
       </c>
-      <c r="D25" s="28">
+      <c r="D25" s="27">
         <f t="shared" si="1"/>
         <v>1009.2923391512256</v>
       </c>
-      <c r="E25" s="37">
+      <c r="E25" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="37">
         <f t="shared" si="2"/>
         <v>61.349142183701943</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="37">
         <f t="shared" si="3"/>
         <v>2.0149974928165371</v>
       </c>
-      <c r="I25" s="30"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="A26" s="21">
         <v>2032</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="22">
         <v>5493.2938067436307</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="23">
         <v>0.51</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <f t="shared" si="1"/>
         <v>1022.5766421253268</v>
       </c>
-      <c r="E26" s="41">
+      <c r="E26" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F26" s="42">
+      <c r="F26" s="41">
         <f t="shared" si="2"/>
         <v>62.156619423304186</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H26" s="42">
+      <c r="H26" s="41">
         <f t="shared" si="3"/>
         <v>2.0415188842393039</v>
       </c>
-      <c r="I26" s="30"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>2033</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="18">
         <v>5565.5965246220849</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="19">
         <v>0.51</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="27">
         <f t="shared" si="1"/>
         <v>1036.0357930584012</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="37">
         <f t="shared" si="2"/>
         <v>62.974724676098901</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="37">
         <f t="shared" si="3"/>
         <v>2.0683893501425632</v>
       </c>
-      <c r="I27" s="30"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="A28" s="21">
         <v>2034</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <v>5638.8508906731167</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="23">
         <v>0.51</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <f t="shared" si="1"/>
         <v>1049.6720932988007</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F28" s="42">
+      <c r="F28" s="41">
         <f t="shared" si="2"/>
         <v>63.803597827966314</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H28" s="42">
+      <c r="H28" s="41">
         <f t="shared" si="3"/>
         <v>2.0956134850436623</v>
       </c>
-      <c r="I28" s="30"/>
+      <c r="I28" s="29"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18">
+      <c r="A29" s="17">
         <v>2035</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="18">
         <v>5709.7470889301703</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="19">
         <v>0.51</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="27">
         <f t="shared" si="1"/>
         <v>1062.8694206043513</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E29" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="37">
         <f t="shared" si="2"/>
         <v>64.605788311244879</v>
       </c>
-      <c r="G29" s="39">
+      <c r="G29" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="37">
         <f t="shared" si="3"/>
         <v>2.1219612342546856</v>
       </c>
-      <c r="I29" s="30"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
+      <c r="A30" s="21">
         <v>2036</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="22">
         <v>5781.5850771845899</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>0.51</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <f t="shared" si="1"/>
         <v>1076.2420621179112</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="41">
         <f t="shared" si="2"/>
         <v>65.41863514834364</v>
       </c>
-      <c r="G30" s="43">
+      <c r="G30" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="41">
         <f t="shared" si="3"/>
         <v>2.1486589887871519</v>
       </c>
-      <c r="I30" s="30"/>
+      <c r="I30" s="29"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="18">
+      <c r="A31" s="17">
         <v>2037</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="18">
         <v>5853.4230654390103</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="19">
         <v>0.51</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="27">
         <f t="shared" si="1"/>
         <v>1089.6147036314719</v>
       </c>
-      <c r="E31" s="37">
+      <c r="E31" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F31" s="38">
+      <c r="F31" s="37">
         <f t="shared" si="2"/>
         <v>66.231481985442414</v>
       </c>
-      <c r="G31" s="39">
+      <c r="G31" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H31" s="38">
+      <c r="H31" s="37">
         <f t="shared" si="3"/>
         <v>2.1753567433196186</v>
       </c>
-      <c r="I31" s="30"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="22">
+      <c r="A32" s="21">
         <v>2038</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <v>5925.2610536934399</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="23">
         <v>0.51</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="28">
         <f t="shared" si="1"/>
         <v>1102.9873451450337</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F32" s="42">
+      <c r="F32" s="41">
         <f t="shared" si="2"/>
         <v>67.04432882254126</v>
       </c>
-      <c r="G32" s="43">
+      <c r="G32" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H32" s="42">
+      <c r="H32" s="41">
         <f t="shared" si="3"/>
         <v>2.2020544978520884</v>
       </c>
-      <c r="I32" s="30"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="18">
+      <c r="A33" s="17">
         <v>2039</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="18">
         <v>5997.0990419478603</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="19">
         <v>0.51</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="27">
         <f t="shared" si="1"/>
         <v>1116.3599866585944</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="36">
         <v>3.1E-2</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="37">
         <f t="shared" si="2"/>
         <v>67.857175659640035</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="38">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="37">
         <f t="shared" si="3"/>
         <v>2.2287522523845551</v>
       </c>
-      <c r="I33" s="30"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
+      <c r="A34" s="21">
         <v>2040</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="22">
         <v>6068.9370302022799</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="23">
         <v>0.51</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="28">
         <f t="shared" si="1"/>
         <v>1129.7326281721544</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="40">
         <v>3.1E-2</v>
       </c>
-      <c r="F34" s="42">
+      <c r="F34" s="41">
         <f t="shared" si="2"/>
         <v>68.670022496738795</v>
       </c>
-      <c r="G34" s="43">
+      <c r="G34" s="42">
         <v>1.0181873788922696E-3</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="43">
         <f t="shared" si="3"/>
         <v>2.2554500069170214</v>
       </c>
-      <c r="I34" s="30"/>
+      <c r="I34" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -6023,117 +6550,117 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="75" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="74" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>46</v>
+      <c r="A1" s="49" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="C2" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="B3" s="53">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="54">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="54">
-        <v>0.34100000000000003</v>
-      </c>
-      <c r="C3" s="53" t="s">
+      <c r="B4" s="56">
+        <v>0.128</v>
+      </c>
+      <c r="C4" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="55">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="D4" s="57">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="57">
-        <v>0.128</v>
-      </c>
-      <c r="C4" s="56" t="s">
+      <c r="B5" s="53">
+        <v>0.13</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="58">
-        <v>2.7E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="D5" s="54">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="54">
-        <v>0.13</v>
-      </c>
-      <c r="C5" s="53" t="s">
+      <c r="B6" s="56">
+        <v>0.114</v>
+      </c>
+      <c r="C6" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="55">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="74" t="s">
+      <c r="D6" s="57">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="57">
-        <v>0.114</v>
-      </c>
-      <c r="C6" s="56" t="s">
+      <c r="B7" s="53">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="54">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="56">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="57"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="58">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="54">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="55">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="57">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="58"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="71"/>
+      <c r="B9" s="70"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="70"/>
+      <c r="D12" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -6155,110 +6682,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>47</v>
+      <c r="A1" s="59" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="C2" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="64">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="65">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="67">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="D4" s="68">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="64">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="65">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="67">
+        <v>0.107</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="68">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="65">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="66">
-        <v>2.3E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="68">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="C4" s="67" t="s">
+      <c r="B7" s="64">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="65">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="67">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C8" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="69">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="65">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="66">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="68">
-        <v>0.107</v>
-      </c>
-      <c r="C6" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="69">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="65">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="66">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="68">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="69">
+      <c r="D8" s="68">
         <v>1.4E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="70"/>
+      <c r="C12" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>